<commit_message>
update to use powerpoint flow
</commit_message>
<xml_diff>
--- a/data/General Table for Post-Colpo/Post-Colpo_LowGrade_Past_HPVnegative_ASCUSorLSIL.xlsx
+++ b/data/General Table for Post-Colpo/Post-Colpo_LowGrade_Past_HPVnegative_ASCUSorLSIL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/egemend2/Documents/Documents/Enduring Guidelines/Web Tool/new tables for the tool/General Table for Post-Colpo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/druss/Downloads/General Table for Post-Colpo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D10FC66B-F1E8-D040-A94F-47BE6E38A63F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CECB071-8263-DE4E-86DB-77A5C6B6FFBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-1960" windowWidth="38400" windowHeight="21600" xr2:uid="{6BB5F710-E77B-364F-B8EF-2549D7586859}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{6BB5F710-E77B-364F-B8EF-2549D7586859}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="118">
   <si>
     <t>N</t>
   </si>
@@ -86,75 +86,21 @@
     <t>CIN2+ Immediate risk (%)</t>
   </si>
   <si>
-    <t>SE immediate</t>
-  </si>
-  <si>
-    <t>LL95 immediate</t>
-  </si>
-  <si>
-    <t>UL95 immediate</t>
-  </si>
-  <si>
     <t>CIN2+ 1 year risk  (%)</t>
   </si>
   <si>
-    <t>SE 1-year</t>
-  </si>
-  <si>
-    <t>LL95 1-year</t>
-  </si>
-  <si>
-    <t>UL95 1-year</t>
-  </si>
-  <si>
     <t>CIN2+ 2 year risk  (%)</t>
   </si>
   <si>
-    <t>SE 2-year</t>
-  </si>
-  <si>
-    <t>LL95 2-year</t>
-  </si>
-  <si>
-    <t>UL95 2-year</t>
-  </si>
-  <si>
     <t>CIN2+ 3 year risk  (%)</t>
   </si>
   <si>
-    <t>SE 3-year</t>
-  </si>
-  <si>
-    <t>LL95 3-year</t>
-  </si>
-  <si>
-    <t>UL95 3-year</t>
-  </si>
-  <si>
     <t>CIN2+ 4 year risk  (%)</t>
   </si>
   <si>
-    <t>SE 4-year</t>
-  </si>
-  <si>
-    <t>LL95 4-year</t>
-  </si>
-  <si>
-    <t>UL95 4-year</t>
-  </si>
-  <si>
     <t>CIN2+ 5 year risk  (%)</t>
   </si>
   <si>
-    <t>SE 5-year</t>
-  </si>
-  <si>
-    <t>LL95 5-year</t>
-  </si>
-  <si>
-    <t>UL95 5-year</t>
-  </si>
-  <si>
     <t>CIN3+ Immediate risk (%)</t>
   </si>
   <si>
@@ -206,9 +152,6 @@
     <t>Unweighted Number of CIN2+ Cases</t>
   </si>
   <si>
-    <t>UnweightedNumber of CIN3+ Cases</t>
-  </si>
-  <si>
     <t>UnweightedNumber of Cancer Cases</t>
   </si>
   <si>
@@ -249,6 +192,204 @@
   </si>
   <si>
     <t xml:space="preserve"> HPV-negative/ASCUS/LSIL</t>
+  </si>
+  <si>
+    <t>CIN2+ SE immediate</t>
+  </si>
+  <si>
+    <t>CIN2+ LL95 immediate</t>
+  </si>
+  <si>
+    <t>CIN2+ UL95 immediate</t>
+  </si>
+  <si>
+    <t>CIN2+ SE 1-year</t>
+  </si>
+  <si>
+    <t>CIN2+ LL95 1-year</t>
+  </si>
+  <si>
+    <t>CIN2+ UL95 1-year</t>
+  </si>
+  <si>
+    <t>CIN2+ SE 2-year</t>
+  </si>
+  <si>
+    <t>CIN2+ LL95 2-year</t>
+  </si>
+  <si>
+    <t>CIN2+ UL95 2-year</t>
+  </si>
+  <si>
+    <t>CIN2+ SE 3-year</t>
+  </si>
+  <si>
+    <t>CIN2+ LL95 3-year</t>
+  </si>
+  <si>
+    <t>CIN2+ UL95 3-year</t>
+  </si>
+  <si>
+    <t>SCIN2+ E 4-year</t>
+  </si>
+  <si>
+    <t>CIN2+ LL95 4-year</t>
+  </si>
+  <si>
+    <t>CIN2+ UL95 4-year</t>
+  </si>
+  <si>
+    <t>CIN2+ SE 5-year</t>
+  </si>
+  <si>
+    <t>CIN2+ LL95 5-year</t>
+  </si>
+  <si>
+    <t>CIN2+ UL95 5-year</t>
+  </si>
+  <si>
+    <t>CIN3+ SE immediate</t>
+  </si>
+  <si>
+    <t>CIN3+ LL95 immediate</t>
+  </si>
+  <si>
+    <t>CIN3+ UL95 immediate</t>
+  </si>
+  <si>
+    <t>CIN3+ SE 1-year</t>
+  </si>
+  <si>
+    <t>CIN3+ LL95 1-year</t>
+  </si>
+  <si>
+    <t>CIN3+ UL95 1-year</t>
+  </si>
+  <si>
+    <t>CIN3+ SE 2-year</t>
+  </si>
+  <si>
+    <t>CIN3+ LL95 2-year</t>
+  </si>
+  <si>
+    <t>CIN3+ UL95 2-year</t>
+  </si>
+  <si>
+    <t>CIN3+ SE 3-year</t>
+  </si>
+  <si>
+    <t>CIN3+ L95 3-year</t>
+  </si>
+  <si>
+    <t>CIN3+ UL95 3-year</t>
+  </si>
+  <si>
+    <t>CIN3+ SE 4-year</t>
+  </si>
+  <si>
+    <t>CIN3+ LL95 4-year</t>
+  </si>
+  <si>
+    <t>CIN3+ UL95 4-year</t>
+  </si>
+  <si>
+    <t>CIN3+ SE 5-year</t>
+  </si>
+  <si>
+    <t>CIN3+ LL95 5-year</t>
+  </si>
+  <si>
+    <t>CIN3+ UL95 5-year</t>
+  </si>
+  <si>
+    <t>CANCER SE immediate</t>
+  </si>
+  <si>
+    <t>CANCER LL95 immediate</t>
+  </si>
+  <si>
+    <t>CANCER UL95 immediate</t>
+  </si>
+  <si>
+    <t>CANCER SE 1-year</t>
+  </si>
+  <si>
+    <t>CANCER LL95 1-year</t>
+  </si>
+  <si>
+    <t>CANCER UL95 1-year</t>
+  </si>
+  <si>
+    <t>CANCER SE 2-year</t>
+  </si>
+  <si>
+    <t>CANCER LL95 2-year</t>
+  </si>
+  <si>
+    <t>CANCER UL95 2-year</t>
+  </si>
+  <si>
+    <t>CANCER SE 3-year</t>
+  </si>
+  <si>
+    <t>CANCER LL95 3-year</t>
+  </si>
+  <si>
+    <t>CANCER UL95 3-year</t>
+  </si>
+  <si>
+    <t>CANCER SE 4-year</t>
+  </si>
+  <si>
+    <t>CANCER LL95 4-year</t>
+  </si>
+  <si>
+    <t>CANCER UL95 4-year</t>
+  </si>
+  <si>
+    <t>CANCER SE 5-year</t>
+  </si>
+  <si>
+    <t>CANCER LL95 5-year</t>
+  </si>
+  <si>
+    <t>CANCER UL95 5-year</t>
+  </si>
+  <si>
+    <t>Unweighted %</t>
+  </si>
+  <si>
+    <t>Unweighted Informative N</t>
+  </si>
+  <si>
+    <t>Unweighted CIN2+ Prevalence Cases</t>
+  </si>
+  <si>
+    <t>Unweighted CIN2+ Incidence Cases</t>
+  </si>
+  <si>
+    <t>Unweighted CIN2+ Unknown Cases</t>
+  </si>
+  <si>
+    <t>Unweighted Number of CIN3+ Cases</t>
+  </si>
+  <si>
+    <t>Unweighted CIN3+ Prevalence Cases</t>
+  </si>
+  <si>
+    <t>Unweighted CIN3+ Incidence Cases</t>
+  </si>
+  <si>
+    <t>Unweighted CIN3+ Unknown Cases</t>
+  </si>
+  <si>
+    <t>Unweighted Cancer Prevalence Cases</t>
+  </si>
+  <si>
+    <t>Unweighted Cancer Incidence Cases</t>
+  </si>
+  <si>
+    <t>Unweighted Cancer Unknown Cases</t>
   </si>
 </sst>
 </file>
@@ -688,10 +829,10 @@
   <dimension ref="A1:DG3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="CI2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD7"/>
+      <selection pane="bottomRight" activeCell="F1" sqref="F1:DF1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -714,19 +855,19 @@
   <sheetData>
     <row r="1" spans="1:111" ht="102" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>0</v>
@@ -777,289 +918,289 @@
         <v>15</v>
       </c>
       <c r="V1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="AH1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AI1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AK1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AL1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AM1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AN1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AO1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AP1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AQ1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AR1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="AS1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AT1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AU1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AV1" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="AW1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AX1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AY1" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AZ1" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="BB1" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="BC1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="BD1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="BE1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="BF1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="BG1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="BH1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="BI1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="BJ1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="BK1" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="BL1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="BM1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AG1" s="5" t="s">
+      <c r="BN1" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="BO1" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="BP1" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="BQ1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="BR1" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="BS1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="BT1" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="BU1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="BV1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="BW1" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="BX1" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="BY1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="BZ1" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="CA1" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="CB1" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="CC1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AK1" s="5" t="s">
+      <c r="CD1" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="CE1" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="CF1" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="CG1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="CH1" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="CI1" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="CJ1" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="CK1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="CL1" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="CM1" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="CN1" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="CO1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="CP1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="AO1" s="5" t="s">
+      <c r="CQ1" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="AP1" s="4" t="s">
+      <c r="CR1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AQ1" s="4" t="s">
+      <c r="CS1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="CT1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="CU1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AR1" s="4" t="s">
+      <c r="CV1" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="CW1" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="CX1" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="CY1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="CZ1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="DA1" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="DB1" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="DC1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AS1" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="AT1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="AU1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="AV1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="AW1" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="AX1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="AY1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="AZ1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="BA1" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="BB1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="BC1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="BD1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="BE1" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="BF1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="BG1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="BH1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="BI1" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="BJ1" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="BK1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="BL1" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="BM1" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="BN1" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="BO1" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="BP1" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="BQ1" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="BR1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="BS1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="BT1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="BU1" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="BV1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="BW1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="BX1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="BY1" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="BZ1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="CA1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="CB1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="CC1" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="CD1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="CE1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="CF1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="CG1" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="CH1" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="CI1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="CJ1" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="CK1" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="CL1" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="CM1" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="CN1" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="CO1" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="CP1" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="CQ1" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="CR1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="CS1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CT1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="CU1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="CV1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="CW1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="CX1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="CY1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="CZ1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="DA1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="DB1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="DC1" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="DD1" s="3" t="s">
-        <v>12</v>
+        <v>115</v>
       </c>
       <c r="DE1" s="3" t="s">
-        <v>13</v>
+        <v>116</v>
       </c>
       <c r="DF1" s="3" t="s">
-        <v>14</v>
+        <v>117</v>
       </c>
       <c r="DG1" s="8"/>
     </row>
     <row r="2" spans="1:111" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="F2" s="13">
         <v>1308</v>
@@ -1321,7 +1462,7 @@
         <v>3.9556591755252801E-7</v>
       </c>
       <c r="CO2" s="10" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="CP2" s="14">
         <v>0.63061296400050038</v>
@@ -1333,19 +1474,19 @@
     </row>
     <row r="3" spans="1:111" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="F3" s="13">
         <v>336</v>
@@ -1607,7 +1748,7 @@
         <v>1.4954046071026E-7</v>
       </c>
       <c r="CO3" s="11" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="CP3" s="14">
         <v>0.81721682434581699</v>

</xml_diff>